<commit_message>
change Man. Planning to Traj. Planning
</commit_message>
<xml_diff>
--- a/data/Dissertation-Evaluation-Prior-Work.xlsx
+++ b/data/Dissertation-Evaluation-Prior-Work.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Desktop\AA_OWN_DISSERTATION\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88107F45-F3A1-4CCF-AD0E-8F26617FD066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="27000" windowHeight="17170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Results" sheetId="1" r:id="rId4"/>
+    <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -196,9 +205,6 @@
     <t>http://dx.doi.org/10.1145/3025171.3025198</t>
   </si>
   <si>
-    <t>Man. Planning</t>
-  </si>
-  <si>
     <t>Car indicators</t>
   </si>
   <si>
@@ -500,27 +506,33 @@
   </si>
   <si>
     <t>Why not</t>
+  </si>
+  <si>
+    <t>Traj. Planning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -528,42 +540,45 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -753,37 +768,42 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:R82"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L49" sqref="L49"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.0"/>
-    <col customWidth="1" min="2" max="2" width="8.0"/>
-    <col customWidth="1" min="3" max="3" width="8.38"/>
-    <col customWidth="1" min="4" max="4" width="8.0"/>
-    <col customWidth="1" min="5" max="5" width="5.38"/>
-    <col customWidth="1" min="6" max="6" width="9.13"/>
-    <col customWidth="1" min="7" max="7" width="10.0"/>
-    <col customWidth="1" min="8" max="8" width="6.25"/>
-    <col customWidth="1" min="9" max="9" width="7.0"/>
-    <col customWidth="1" min="10" max="10" width="12.75"/>
-    <col customWidth="1" min="11" max="11" width="5.5"/>
-    <col customWidth="1" min="12" max="12" width="10.25"/>
-    <col customWidth="1" min="13" max="13" width="5.25"/>
-    <col customWidth="1" min="15" max="15" width="24.25"/>
-    <col customWidth="1" min="16" max="16" width="43.38"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="8.36328125" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="5.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.08984375" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="6.26953125" customWidth="1"/>
+    <col min="9" max="9" width="7" customWidth="1"/>
+    <col min="10" max="10" width="12.7265625" customWidth="1"/>
+    <col min="11" max="11" width="5.453125" customWidth="1"/>
+    <col min="12" max="12" width="10.26953125" customWidth="1"/>
+    <col min="13" max="13" width="5.26953125" customWidth="1"/>
+    <col min="15" max="15" width="24.26953125" customWidth="1"/>
+    <col min="16" max="16" width="43.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -833,7 +853,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -854,7 +874,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -875,7 +895,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -892,22 +912,22 @@
         <v>1.41</v>
       </c>
       <c r="F4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H4" s="1">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="I4" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K4" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>19</v>
@@ -922,7 +942,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -939,22 +959,22 @@
         <v>1.08</v>
       </c>
       <c r="F5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="I5" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>19</v>
@@ -969,7 +989,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -987,7 +1007,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1004,22 +1024,22 @@
         <v>1.3</v>
       </c>
       <c r="F7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H7" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="I7" s="1">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K7" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>19</v>
@@ -1034,7 +1054,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -1051,22 +1071,22 @@
         <v>1.41</v>
       </c>
       <c r="F8" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H8" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="I8" s="1">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K8" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>19</v>
@@ -1081,7 +1101,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -1095,7 +1115,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1106,7 +1126,7 @@
         <v>18</v>
       </c>
       <c r="I10" s="1">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>19</v>
@@ -1118,7 +1138,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -1138,12 +1158,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
       <c r="I12" s="1">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>19</v>
@@ -1155,7 +1175,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -1172,22 +1192,22 @@
         <v>1.7</v>
       </c>
       <c r="F13" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H13" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="I13" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K13" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>19</v>
@@ -1199,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
@@ -1210,28 +1230,28 @@
         <v>18</v>
       </c>
       <c r="D14" s="1">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E14" s="1">
         <v>1.8</v>
       </c>
       <c r="F14" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H14" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="I14" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K14" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>19</v>
@@ -1243,7 +1263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -1260,22 +1280,22 @@
         <v>1.2</v>
       </c>
       <c r="F15" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H15" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="I15" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K15" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>19</v>
@@ -1287,7 +1307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -1310,7 +1330,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>49</v>
       </c>
@@ -1330,7 +1350,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
@@ -1341,19 +1361,19 @@
         <v>18</v>
       </c>
       <c r="F18" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H18" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="I18" s="1">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="K18" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>19</v>
@@ -1365,7 +1385,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
@@ -1382,22 +1402,22 @@
         <v>0.67</v>
       </c>
       <c r="F19" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H19" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="I19" s="1">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K19" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>19</v>
@@ -1412,7 +1432,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
@@ -1429,22 +1449,22 @@
         <v>0.91</v>
       </c>
       <c r="F20" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H20" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="I20" s="1">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>58</v>
       </c>
       <c r="K20" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>19</v>
@@ -1459,7 +1479,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>59</v>
       </c>
@@ -1473,37 +1493,37 @@
         <v>2.4</v>
       </c>
       <c r="F21" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G21" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H21" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="I21" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K21" s="1">
+        <v>5</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K21" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N21" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22">
+    </row>
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>59</v>
       </c>
@@ -1517,22 +1537,22 @@
         <v>2.7</v>
       </c>
       <c r="F22" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G22" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H22" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="I22" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K22" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>19</v>
@@ -1544,10 +1564,10 @@
         <v>0</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>59</v>
       </c>
@@ -1561,22 +1581,22 @@
         <v>2.9</v>
       </c>
       <c r="F23" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G23" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H23" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="I23" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K23" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>19</v>
@@ -1588,15 +1608,15 @@
         <v>0</v>
       </c>
       <c r="P23" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>18</v>
@@ -1605,22 +1625,22 @@
         <v>3.91</v>
       </c>
       <c r="F24" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H24" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="I24" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K24" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>19</v>
@@ -1632,59 +1652,59 @@
         <v>0</v>
       </c>
       <c r="P24" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>7</v>
+      </c>
+      <c r="H25" s="1">
+        <v>2019</v>
+      </c>
+      <c r="I25" s="1">
+        <v>30</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K25" s="1">
+        <v>5</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P25" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="1">
-        <v>5.06</v>
-      </c>
-      <c r="F25" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="G25" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="H25" s="1">
-        <v>2019.0</v>
-      </c>
-      <c r="I25" s="1">
-        <v>30.0</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K25" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N25" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>18</v>
@@ -1693,22 +1713,22 @@
         <v>4.2</v>
       </c>
       <c r="F26" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H26" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="I26" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K26" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>19</v>
@@ -1720,15 +1740,15 @@
         <v>0</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>18</v>
@@ -1737,22 +1757,22 @@
         <v>4.79</v>
       </c>
       <c r="F27" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H27" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="I27" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K27" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>19</v>
@@ -1764,15 +1784,15 @@
         <v>0</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>18</v>
@@ -1781,22 +1801,22 @@
         <v>4.75</v>
       </c>
       <c r="F28" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H28" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="I28" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K28" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>19</v>
@@ -1808,15 +1828,15 @@
         <v>0</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>18</v>
@@ -1825,22 +1845,22 @@
         <v>4.79</v>
       </c>
       <c r="F29" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H29" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="I29" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K29" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>19</v>
@@ -1852,15 +1872,15 @@
         <v>0</v>
       </c>
       <c r="P29" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>18</v>
@@ -1872,42 +1892,42 @@
         <v>0.76</v>
       </c>
       <c r="F30" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H30" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="I30" s="1">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K30" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>19</v>
       </c>
       <c r="M30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="N30" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31">
+    </row>
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>18</v>
@@ -1919,42 +1939,42 @@
         <v>0.75</v>
       </c>
       <c r="F31" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H31" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="I31" s="1">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K31" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P31" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M31" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N31" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="P31" s="1" t="s">
+    </row>
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>18</v>
@@ -1966,39 +1986,39 @@
         <v>1.46</v>
       </c>
       <c r="F32" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G32" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H32" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="I32" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K32" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>19</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N32" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>18</v>
@@ -2010,42 +2030,42 @@
         <v>1.86</v>
       </c>
       <c r="F33" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H33" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="I33" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="J33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K33" s="1">
+        <v>5</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P33" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K33" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N33" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="P33" s="1" t="s">
+    </row>
+    <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>29</v>
@@ -2057,39 +2077,39 @@
         <v>0.96</v>
       </c>
       <c r="F34" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H34" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="I34" s="1">
-        <v>216.0</v>
+        <v>216</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K34" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>19</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N34" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>29</v>
@@ -2101,42 +2121,42 @@
         <v>0.92</v>
       </c>
       <c r="F35" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H35" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="I35" s="1">
-        <v>216.0</v>
+        <v>216</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K35" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N35" s="1" t="b">
         <v>0</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>29</v>
@@ -2148,42 +2168,42 @@
         <v>1.19</v>
       </c>
       <c r="F36" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G36" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H36" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="I36" s="1">
-        <v>216.0</v>
+        <v>216</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K36" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N36" s="1" t="b">
         <v>0</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>29</v>
@@ -2195,100 +2215,100 @@
         <v>1.08</v>
       </c>
       <c r="F37" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H37" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="I37" s="1">
-        <v>216.0</v>
+        <v>216</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="K37" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N37" s="1" t="b">
         <v>0</v>
       </c>
       <c r="P37" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H38" s="1">
+        <v>2022</v>
+      </c>
+      <c r="I38" s="1">
+        <v>18</v>
+      </c>
+      <c r="K38" s="1">
+        <v>5</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N38" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O38" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H38" s="1">
-        <v>2022.0</v>
-      </c>
-      <c r="I38" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="K38" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N38" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="O38" s="1" t="s">
+    </row>
+    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H39" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="K39" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>19</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N39" s="1" t="b">
         <v>1</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>29</v>
@@ -2300,39 +2320,39 @@
         <v>0.78</v>
       </c>
       <c r="F40" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H40" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="I40" s="1">
-        <v>280.0</v>
+        <v>280</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="K40" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L40" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N40" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P40" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N40" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41">
+    </row>
+    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>29</v>
@@ -2344,39 +2364,39 @@
         <v>0.9</v>
       </c>
       <c r="F41" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H41" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="I41" s="1">
-        <v>280.0</v>
+        <v>280</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K41" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L41" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N41" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P41" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M41" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N41" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42">
+    </row>
+    <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>29</v>
@@ -2388,39 +2408,39 @@
         <v>0.79</v>
       </c>
       <c r="F42" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G42" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H42" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="I42" s="1">
-        <v>280.0</v>
+        <v>280</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K42" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L42" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N42" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P42" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M42" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N42" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="P42" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43">
+    </row>
+    <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>29</v>
@@ -2432,66 +2452,66 @@
         <v>0.91</v>
       </c>
       <c r="F43" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H43" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="I43" s="1">
-        <v>280.0</v>
+        <v>280</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K43" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>19</v>
       </c>
       <c r="M43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N43" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P43" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="N43" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="P43" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44">
+    </row>
+    <row r="44" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="C44" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D44" s="1">
-        <v>4.23</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="F44" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H44" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="I44" s="1">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K44" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>19</v>
@@ -2503,18 +2523,18 @@
         <v>0</v>
       </c>
       <c r="P44" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q44" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="Q44" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45">
+    </row>
+    <row r="45" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>18</v>
@@ -2523,22 +2543,22 @@
         <v>3.48</v>
       </c>
       <c r="F45" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G45" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H45" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="I45" s="1">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K45" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>19</v>
@@ -2550,18 +2570,18 @@
         <v>0</v>
       </c>
       <c r="P45" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q45" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="Q45" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46">
+    </row>
+    <row r="46" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>18</v>
@@ -2570,22 +2590,22 @@
         <v>4.05</v>
       </c>
       <c r="F46" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H46" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="I46" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="K46" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>19</v>
@@ -2597,18 +2617,18 @@
         <v>0</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>18</v>
@@ -2617,22 +2637,22 @@
         <v>3.21</v>
       </c>
       <c r="F47" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G47" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H47" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="I47" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="K47" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L47" s="1" t="s">
         <v>19</v>
@@ -2644,42 +2664,42 @@
         <v>0</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="C48" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D48" s="1">
-        <v>2.47</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="F48" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G48" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H48" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="I48" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K48" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L48" s="1" t="s">
         <v>19</v>
@@ -2691,38 +2711,38 @@
         <v>0</v>
       </c>
       <c r="P48" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q48" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="s">
+      <c r="B49" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="L49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N49" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O49" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="L49" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M49" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N49" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="O49" s="1" t="s">
+    </row>
+    <row r="50" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="s">
+      <c r="B50" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>18</v>
@@ -2734,45 +2754,45 @@
         <v>1.42</v>
       </c>
       <c r="F50" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G50" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H50" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="I50" s="1">
-        <v>68.0</v>
+        <v>68</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K50" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N50" s="1" t="b">
         <v>0</v>
       </c>
       <c r="P50" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="s">
+      <c r="B51" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="D51" s="1">
         <v>60.4</v>
@@ -2781,22 +2801,22 @@
         <v>7.9</v>
       </c>
       <c r="F51" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G51" s="1">
-        <v>84.0</v>
+        <v>84</v>
       </c>
       <c r="H51" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="I51" s="1">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K51" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>19</v>
@@ -2808,15 +2828,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="D52" s="1">
         <v>64.92</v>
@@ -2825,22 +2845,22 @@
         <v>9.51</v>
       </c>
       <c r="F52" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G52" s="1">
-        <v>84.0</v>
+        <v>84</v>
       </c>
       <c r="H52" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="I52" s="1">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K52" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>19</v>
@@ -2852,45 +2872,45 @@
         <v>0</v>
       </c>
       <c r="P52" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q52" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Q52" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="53">
+    </row>
+    <row r="53" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D53" s="1">
-        <v>64.04</v>
+        <v>64.040000000000006</v>
       </c>
       <c r="E53" s="1">
-        <v>10.22</v>
+        <v>10.220000000000001</v>
       </c>
       <c r="F53" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G53" s="1">
-        <v>84.0</v>
+        <v>84</v>
       </c>
       <c r="H53" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="I53" s="1">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K53" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>19</v>
@@ -2902,45 +2922,45 @@
         <v>0</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="54">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D54" s="1">
-        <v>65.96</v>
+        <v>65.959999999999994</v>
       </c>
       <c r="E54" s="1">
         <v>8.07</v>
       </c>
       <c r="F54" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G54" s="1">
-        <v>84.0</v>
+        <v>84</v>
       </c>
       <c r="H54" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="I54" s="1">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K54" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>19</v>
@@ -2952,41 +2972,41 @@
         <v>0</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q54" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="s">
+      <c r="B55" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="K55" s="1">
+        <v>2</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N55" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O55" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="K55" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M55" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N55" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="O55" s="1" t="s">
+    </row>
+    <row r="56" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="s">
+      <c r="B56" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>18</v>
@@ -2998,22 +3018,22 @@
         <v>0.5</v>
       </c>
       <c r="F56" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G56" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H56" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="I56" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K56" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L56" s="1" t="s">
         <v>19</v>
@@ -3025,21 +3045,21 @@
         <v>0</v>
       </c>
       <c r="P56" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q56" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="Q56" s="1" t="s">
+      <c r="R56" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="R56" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="57">
+    </row>
+    <row r="57" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>18</v>
@@ -3051,22 +3071,22 @@
         <v>0.5</v>
       </c>
       <c r="F57" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G57" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H57" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="I57" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K57" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>19</v>
@@ -3078,48 +3098,48 @@
         <v>0</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q57" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="R57" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="R57" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="58">
+    </row>
+    <row r="58" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="C58" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D58" s="1">
-        <v>4.15</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="E58" s="1">
         <v>0.5</v>
       </c>
       <c r="F58" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G58" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H58" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="I58" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K58" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L58" s="1" t="s">
         <v>19</v>
@@ -3131,21 +3151,21 @@
         <v>0</v>
       </c>
       <c r="P58" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q58" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="R58" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="Q58" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="R58" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="s">
+      <c r="B59" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>18</v>
@@ -3154,25 +3174,25 @@
         <v>3.5</v>
       </c>
       <c r="E59" s="1">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F59" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G59" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H59" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="I59" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K59" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>19</v>
@@ -3184,15 +3204,15 @@
         <v>0</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="60">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>18</v>
@@ -3204,22 +3224,22 @@
         <v>1.2</v>
       </c>
       <c r="F60" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G60" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H60" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="I60" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K60" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L60" s="1" t="s">
         <v>19</v>
@@ -3231,15 +3251,15 @@
         <v>0</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="61">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>18</v>
@@ -3248,28 +3268,28 @@
         <v>3.4</v>
       </c>
       <c r="E61" s="1">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F61" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G61" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H61" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="I61" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K61" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M61" s="1" t="s">
         <v>19</v>
@@ -3278,42 +3298,42 @@
         <v>0</v>
       </c>
       <c r="P61" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q61" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="Q61" s="1" t="s">
+    </row>
+    <row r="62" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="s">
+      <c r="B62" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="D62" s="1">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F62" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G62" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H62" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="I62" s="1">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K62" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L62" s="1" t="s">
         <v>19</v>
@@ -3325,39 +3345,39 @@
         <v>0</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="63">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="D63" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F63" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G63" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H63" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="I63" s="1">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="J63" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K63" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L63" s="1" t="s">
         <v>19</v>
@@ -3369,36 +3389,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="D64" s="1">
         <v>3.8</v>
       </c>
       <c r="F64" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G64" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H64" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="I64" s="1">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K64" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L64" s="1" t="s">
         <v>19</v>
@@ -3410,18 +3430,18 @@
         <v>0</v>
       </c>
       <c r="P64" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="D65" s="1">
         <v>3.84</v>
@@ -3430,22 +3450,22 @@
         <v>0.7</v>
       </c>
       <c r="F65" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G65" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H65" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="I65" s="1">
-        <v>216.0</v>
+        <v>216</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K65" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>19</v>
@@ -3457,21 +3477,21 @@
         <v>0</v>
       </c>
       <c r="P65" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q65" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="Q65" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="66">
+    </row>
+    <row r="66" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="D66" s="1">
         <v>3.57</v>
@@ -3480,22 +3500,22 @@
         <v>0.69</v>
       </c>
       <c r="F66" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G66" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H66" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="I66" s="1">
-        <v>216.0</v>
+        <v>216</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K66" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>19</v>
@@ -3507,21 +3527,21 @@
         <v>0</v>
       </c>
       <c r="P66" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q66" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="Q66" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="s">
+      <c r="B67" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="D67" s="1">
         <v>5.41</v>
@@ -3530,22 +3550,22 @@
         <v>0.87</v>
       </c>
       <c r="F67" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G67" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H67" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="I67" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="J67" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K67" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>19</v>
@@ -3557,39 +3577,39 @@
         <v>0</v>
       </c>
       <c r="P67" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="1" t="s">
+      <c r="B68" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="C68" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D68" s="1">
         <v>2.63</v>
       </c>
       <c r="F68" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G68" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H68" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="I68" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K68" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L68" s="1" t="s">
         <v>19</v>
@@ -3601,39 +3621,39 @@
         <v>0</v>
       </c>
       <c r="P68" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="69">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="C69" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D69" s="1">
         <v>3.6</v>
       </c>
       <c r="F69" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G69" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H69" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="I69" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K69" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L69" s="1" t="s">
         <v>19</v>
@@ -3645,39 +3665,39 @@
         <v>0</v>
       </c>
       <c r="P69" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="70">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="C70" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D70" s="1">
         <v>3.53</v>
       </c>
       <c r="F70" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G70" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H70" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="I70" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K70" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L70" s="1" t="s">
         <v>19</v>
@@ -3689,15 +3709,15 @@
         <v>0</v>
       </c>
       <c r="P70" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="s">
+      <c r="B71" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>18</v>
@@ -3706,25 +3726,25 @@
         <v>4.99</v>
       </c>
       <c r="E71" s="1">
-        <v>1.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="F71" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G71" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H71" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="I71" s="1">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K71" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L71" s="1" t="s">
         <v>19</v>
@@ -3736,18 +3756,18 @@
         <v>0</v>
       </c>
       <c r="P71" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q71" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="Q71" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="72">
+    </row>
+    <row r="72" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>18</v>
@@ -3759,22 +3779,22 @@
         <v>1.2</v>
       </c>
       <c r="F72" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G72" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H72" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="I72" s="1">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K72" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L72" s="1" t="s">
         <v>19</v>
@@ -3786,18 +3806,18 @@
         <v>0</v>
       </c>
       <c r="P72" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Q72" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="73">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>18</v>
@@ -3809,22 +3829,22 @@
         <v>1.21</v>
       </c>
       <c r="F73" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G73" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H73" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="I73" s="1">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K73" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L73" s="1" t="s">
         <v>19</v>
@@ -3836,45 +3856,45 @@
         <v>0</v>
       </c>
       <c r="P73" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q73" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="Q73" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D74" s="1">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E74" s="1">
         <v>0.25</v>
       </c>
       <c r="F74" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G74" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H74" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="I74" s="1">
-        <v>340.0</v>
+        <v>340</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K74" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L74" s="1" t="s">
         <v>19</v>
@@ -3886,45 +3906,45 @@
         <v>0</v>
       </c>
       <c r="P74" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q74" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="Q74" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="75">
+    </row>
+    <row r="75" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D75" s="1">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E75" s="1">
         <v>0.25</v>
       </c>
       <c r="F75" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G75" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H75" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="I75" s="1">
-        <v>340.0</v>
+        <v>340</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K75" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L75" s="1" t="s">
         <v>19</v>
@@ -3936,45 +3956,45 @@
         <v>0</v>
       </c>
       <c r="P75" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q75" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="Q75" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="76">
+    </row>
+    <row r="76" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D76" s="1">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E76" s="1">
         <v>0.25</v>
       </c>
       <c r="F76" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G76" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H76" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="I76" s="1">
-        <v>340.0</v>
+        <v>340</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K76" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L76" s="1" t="s">
         <v>19</v>
@@ -3986,45 +4006,45 @@
         <v>0</v>
       </c>
       <c r="P76" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q76" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="77">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D77" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E77" s="1">
         <v>0.25</v>
       </c>
       <c r="F77" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G77" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H77" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="I77" s="1">
-        <v>340.0</v>
+        <v>340</v>
       </c>
       <c r="J77" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K77" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L77" s="1" t="s">
         <v>19</v>
@@ -4036,56 +4056,56 @@
         <v>0</v>
       </c>
       <c r="P77" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q77" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="Q77" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="s">
+      <c r="B78" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="C78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F78" s="1">
+        <v>1</v>
+      </c>
+      <c r="G78" s="1">
+        <v>5</v>
+      </c>
+      <c r="H78" s="1">
+        <v>2023</v>
+      </c>
+      <c r="I78" s="1">
+        <v>113</v>
+      </c>
+      <c r="K78" s="1">
+        <v>4</v>
+      </c>
+      <c r="L78" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N78" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P78" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F78" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="G78" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="H78" s="1">
-        <v>2023.0</v>
-      </c>
-      <c r="I78" s="1">
-        <v>113.0</v>
-      </c>
-      <c r="K78" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="L78" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M78" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N78" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="P78" s="1" t="s">
+    </row>
+    <row r="79" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="s">
+      <c r="B79" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>29</v>
@@ -4097,22 +4117,22 @@
         <v>0.5</v>
       </c>
       <c r="F79" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G79" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H79" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="I79" s="1">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="J79" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K79" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L79" s="1" t="s">
         <v>19</v>
@@ -4124,18 +4144,18 @@
         <v>0</v>
       </c>
       <c r="P79" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q79" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="Q79" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="80">
+    </row>
+    <row r="80" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>29</v>
@@ -4147,22 +4167,22 @@
         <v>0.4</v>
       </c>
       <c r="F80" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G80" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H80" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="I80" s="1">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="J80" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K80" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L80" s="1" t="s">
         <v>19</v>
@@ -4174,45 +4194,45 @@
         <v>0</v>
       </c>
       <c r="P80" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Q80" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="81">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D81" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E81" s="1">
         <v>0.5</v>
       </c>
       <c r="F81" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G81" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H81" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="I81" s="1">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="J81" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K81" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L81" s="1" t="s">
         <v>19</v>
@@ -4224,18 +4244,18 @@
         <v>0</v>
       </c>
       <c r="P81" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q81" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="82">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>29</v>
@@ -4247,22 +4267,22 @@
         <v>0.5</v>
       </c>
       <c r="F82" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G82" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H82" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="I82" s="1">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K82" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L82" s="1" t="s">
         <v>19</v>
@@ -4274,83 +4294,83 @@
         <v>0</v>
       </c>
       <c r="P82" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q82" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B7"/>
-    <hyperlink r:id="rId6" ref="B8"/>
-    <hyperlink r:id="rId7" ref="B10"/>
-    <hyperlink r:id="rId8" ref="B11"/>
-    <hyperlink r:id="rId9" ref="B13"/>
-    <hyperlink r:id="rId10" ref="B14"/>
-    <hyperlink r:id="rId11" ref="B15"/>
-    <hyperlink r:id="rId12" ref="B16"/>
-    <hyperlink r:id="rId13" ref="B17"/>
-    <hyperlink r:id="rId14" ref="B18"/>
-    <hyperlink r:id="rId15" ref="B19"/>
-    <hyperlink r:id="rId16" ref="B20"/>
-    <hyperlink r:id="rId17" ref="B21"/>
-    <hyperlink r:id="rId18" ref="B22"/>
-    <hyperlink r:id="rId19" ref="B23"/>
-    <hyperlink r:id="rId20" ref="B24"/>
-    <hyperlink r:id="rId21" ref="B25"/>
-    <hyperlink r:id="rId22" ref="B26"/>
-    <hyperlink r:id="rId23" ref="B27"/>
-    <hyperlink r:id="rId24" ref="B28"/>
-    <hyperlink r:id="rId25" ref="B29"/>
-    <hyperlink r:id="rId26" ref="B30"/>
-    <hyperlink r:id="rId27" ref="B31"/>
-    <hyperlink r:id="rId28" ref="B32"/>
-    <hyperlink r:id="rId29" ref="B33"/>
-    <hyperlink r:id="rId30" ref="B34"/>
-    <hyperlink r:id="rId31" ref="B35"/>
-    <hyperlink r:id="rId32" ref="B36"/>
-    <hyperlink r:id="rId33" ref="B37"/>
-    <hyperlink r:id="rId34" ref="B38"/>
-    <hyperlink r:id="rId35" ref="B39"/>
-    <hyperlink r:id="rId36" ref="B44"/>
-    <hyperlink r:id="rId37" ref="B45"/>
-    <hyperlink r:id="rId38" ref="B46"/>
-    <hyperlink r:id="rId39" ref="B47"/>
-    <hyperlink r:id="rId40" ref="B48"/>
-    <hyperlink r:id="rId41" ref="B49"/>
-    <hyperlink r:id="rId42" ref="B50"/>
-    <hyperlink r:id="rId43" ref="B51"/>
-    <hyperlink r:id="rId44" ref="B52"/>
-    <hyperlink r:id="rId45" ref="B53"/>
-    <hyperlink r:id="rId46" ref="B54"/>
-    <hyperlink r:id="rId47" ref="B55"/>
-    <hyperlink r:id="rId48" ref="B56"/>
-    <hyperlink r:id="rId49" ref="B57"/>
-    <hyperlink r:id="rId50" ref="B58"/>
-    <hyperlink r:id="rId51" ref="B59"/>
-    <hyperlink r:id="rId52" ref="B60"/>
-    <hyperlink r:id="rId53" ref="B61"/>
-    <hyperlink r:id="rId54" ref="B62"/>
-    <hyperlink r:id="rId55" ref="B63"/>
-    <hyperlink r:id="rId56" ref="B64"/>
-    <hyperlink r:id="rId57" ref="B67"/>
-    <hyperlink r:id="rId58" ref="B68"/>
-    <hyperlink r:id="rId59" ref="B69"/>
-    <hyperlink r:id="rId60" ref="B70"/>
-    <hyperlink r:id="rId61" ref="B71"/>
-    <hyperlink r:id="rId62" ref="B72"/>
-    <hyperlink r:id="rId63" ref="B73"/>
-    <hyperlink r:id="rId64" ref="B78"/>
-    <hyperlink r:id="rId65" ref="B79"/>
-    <hyperlink r:id="rId66" ref="B80"/>
-    <hyperlink r:id="rId67" ref="B81"/>
-    <hyperlink r:id="rId68" ref="B82"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B25" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B27" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B28" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B29" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B30" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B31" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B32" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B33" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B34" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B35" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B36" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B37" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B38" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B39" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B44" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B45" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B46" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B47" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B48" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B49" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B50" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B51" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B52" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B53" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B54" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B55" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B56" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B57" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B58" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B59" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B60" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B61" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B62" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B63" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B64" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B67" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B68" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B69" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B70" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B71" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B72" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B73" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B78" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B79" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B80" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B81" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B82" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
   </hyperlinks>
-  <drawing r:id="rId69"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>